<commit_message>
Updated by Artyom Borisov 10.01.2023
</commit_message>
<xml_diff>
--- a/СтатГрад/2022-12/files/22.xlsx
+++ b/СтатГрад/2022-12/files/22.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ЕГЭ\2023\2022-12 ТР2\Решения\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79686\Desktop\EGE_2023\СтатГрад\2022-12\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2118FD-7E5D-4960-A83D-39E2C408FD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30510" yWindow="2070" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -132,7 +131,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -453,21 +452,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="62.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -479,7 +478,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>10026</v>
       </c>
@@ -491,7 +490,7 @@
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>10123</v>
       </c>
@@ -503,7 +502,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>10208</v>
       </c>
@@ -513,8 +512,9 @@
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>10218</v>
       </c>
@@ -526,7 +526,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>10251</v>
       </c>
@@ -538,7 +538,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>10285</v>
       </c>
@@ -550,7 +550,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>10374</v>
       </c>
@@ -562,7 +562,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>10423</v>
       </c>
@@ -574,7 +574,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>10495</v>
       </c>
@@ -586,7 +586,7 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10594</v>
       </c>
@@ -598,7 +598,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>10629</v>
       </c>
@@ -610,7 +610,7 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>10707</v>
       </c>
@@ -622,7 +622,7 @@
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>10746</v>
       </c>
@@ -632,8 +632,9 @@
       <c r="C14" s="3">
         <v>10707</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>10824</v>
       </c>
@@ -643,8 +644,9 @@
       <c r="C15" s="3">
         <v>10123</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>10856</v>
       </c>
@@ -654,8 +656,9 @@
       <c r="C16" s="3">
         <v>10707</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>10954</v>
       </c>
@@ -665,8 +668,9 @@
       <c r="C17" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>10980</v>
       </c>
@@ -676,8 +680,9 @@
       <c r="C18" s="3">
         <v>10824</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>10994</v>
       </c>
@@ -687,8 +692,9 @@
       <c r="C19" s="3">
         <v>10594</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>11040</v>
       </c>
@@ -698,8 +704,9 @@
       <c r="C20" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>11125</v>
       </c>
@@ -709,8 +716,9 @@
       <c r="C21" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>11177</v>
       </c>
@@ -720,8 +728,9 @@
       <c r="C22" s="3">
         <v>10026</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>11229</v>
       </c>
@@ -731,8 +740,9 @@
       <c r="C23" s="3">
         <v>10856</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>11245</v>
       </c>
@@ -742,8 +752,9 @@
       <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>11324</v>
       </c>
@@ -753,8 +764,9 @@
       <c r="C25" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>11422</v>
       </c>
@@ -764,8 +776,9 @@
       <c r="C26" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>11502</v>
       </c>
@@ -775,8 +788,9 @@
       <c r="C27" s="3">
         <v>10374</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>11593</v>
       </c>
@@ -786,8 +800,9 @@
       <c r="C28" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>11612</v>
       </c>
@@ -797,8 +812,9 @@
       <c r="C29" s="3">
         <v>10026</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>11680</v>
       </c>
@@ -808,8 +824,9 @@
       <c r="C30" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>11742</v>
       </c>
@@ -819,8 +836,9 @@
       <c r="C31" s="3">
         <v>10629</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>11777</v>
       </c>
@@ -830,8 +848,9 @@
       <c r="C32" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>11842</v>
       </c>
@@ -841,8 +860,9 @@
       <c r="C33" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>11930</v>
       </c>
@@ -852,8 +872,9 @@
       <c r="C34" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>11971</v>
       </c>
@@ -863,8 +884,9 @@
       <c r="C35" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>12024</v>
       </c>
@@ -874,8 +896,9 @@
       <c r="C36" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>12107</v>
       </c>
@@ -885,8 +908,9 @@
       <c r="C37" s="3">
         <v>11177</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>12201</v>
       </c>
@@ -896,8 +920,9 @@
       <c r="C38" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>12299</v>
       </c>
@@ -907,8 +932,9 @@
       <c r="C39" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>12344</v>
       </c>
@@ -918,8 +944,9 @@
       <c r="C40" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>12371</v>
       </c>
@@ -929,8 +956,9 @@
       <c r="C41" s="3">
         <v>11502</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>12380</v>
       </c>
@@ -940,8 +968,9 @@
       <c r="C42" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>12460</v>
       </c>
@@ -951,8 +980,9 @@
       <c r="C43" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>12521</v>
       </c>
@@ -962,8 +992,9 @@
       <c r="C44" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>12607</v>
       </c>
@@ -973,8 +1004,9 @@
       <c r="C45" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>12690</v>
       </c>
@@ -984,8 +1016,9 @@
       <c r="C46" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>12783</v>
       </c>
@@ -995,8 +1028,9 @@
       <c r="C47" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>12804</v>
       </c>
@@ -1006,8 +1040,9 @@
       <c r="C48" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>12858</v>
       </c>
@@ -1017,8 +1052,9 @@
       <c r="C49" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>12931</v>
       </c>
@@ -1028,8 +1064,9 @@
       <c r="C50" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>13015</v>
       </c>
@@ -1039,8 +1076,9 @@
       <c r="C51" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>13097</v>
       </c>
@@ -1050,8 +1088,9 @@
       <c r="C52" s="3">
         <v>11612</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>13159</v>
       </c>
@@ -1061,8 +1100,9 @@
       <c r="C53" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>13237</v>
       </c>
@@ -1072,8 +1112,9 @@
       <c r="C54" s="3">
         <v>12024</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>13265</v>
       </c>
@@ -1083,8 +1124,9 @@
       <c r="C55" s="3">
         <v>12024</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>13280</v>
       </c>
@@ -1094,8 +1136,9 @@
       <c r="C56" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>13340</v>
       </c>
@@ -1105,8 +1148,9 @@
       <c r="C57" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>13375</v>
       </c>
@@ -1116,8 +1160,9 @@
       <c r="C58" s="3">
         <v>12107</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>13378</v>
       </c>
@@ -1127,8 +1172,9 @@
       <c r="C59" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>13391</v>
       </c>
@@ -1138,8 +1184,9 @@
       <c r="C60" s="3">
         <v>10423</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>13421</v>
       </c>
@@ -1149,8 +1196,9 @@
       <c r="C61" s="3">
         <v>10374</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>13440</v>
       </c>
@@ -1160,8 +1208,9 @@
       <c r="C62" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>13520</v>
       </c>
@@ -1171,8 +1220,9 @@
       <c r="C63" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>13523</v>
       </c>
@@ -1182,8 +1232,9 @@
       <c r="C64" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D64" s="3"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>13613</v>
       </c>
@@ -1193,8 +1244,9 @@
       <c r="C65" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>13658</v>
       </c>
@@ -1204,8 +1256,9 @@
       <c r="C66" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D66" s="3"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>13720</v>
       </c>
@@ -1215,8 +1268,9 @@
       <c r="C67" s="3">
         <v>11422</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>13734</v>
       </c>
@@ -1226,8 +1280,9 @@
       <c r="C68" s="3">
         <v>13280</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D68" s="3"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>13799</v>
       </c>
@@ -1237,8 +1292,9 @@
       <c r="C69" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D69" s="3"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>13877</v>
       </c>
@@ -1248,8 +1304,9 @@
       <c r="C70" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D70" s="3"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>13892</v>
       </c>
@@ -1259,8 +1316,9 @@
       <c r="C71" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D71" s="3"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>13896</v>
       </c>
@@ -1270,325 +1328,331 @@
       <c r="C72" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D72" s="3"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
-        <v>13896</v>
+        <v>13952</v>
       </c>
       <c r="B73" s="3">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="C73" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
-        <v>13952</v>
+        <v>13985</v>
       </c>
       <c r="B74" s="3">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C74" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+        <v>11842</v>
+      </c>
+      <c r="D74" s="3"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
-        <v>13985</v>
+        <v>14011</v>
       </c>
       <c r="B75" s="3">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C75" s="3">
-        <v>11842</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="D75" s="3"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
-        <v>14011</v>
+        <v>14033</v>
       </c>
       <c r="B76" s="3">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="C76" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D76" s="3"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
-        <v>14033</v>
+        <v>14115</v>
       </c>
       <c r="B77" s="3">
+        <v>25</v>
+      </c>
+      <c r="C77" s="3">
+        <v>11930</v>
+      </c>
+      <c r="D77" s="3"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="3">
+        <v>14187</v>
+      </c>
+      <c r="B78" s="3">
+        <v>42</v>
+      </c>
+      <c r="C78" s="3">
+        <v>0</v>
+      </c>
+      <c r="D78" s="3"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="3">
+        <v>14255</v>
+      </c>
+      <c r="B79" s="3">
+        <v>93</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D79" s="3"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="3">
+        <v>14301</v>
+      </c>
+      <c r="B80" s="3">
+        <v>81</v>
+      </c>
+      <c r="C80" s="3">
+        <v>0</v>
+      </c>
+      <c r="D80" s="3"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="3">
+        <v>14336</v>
+      </c>
+      <c r="B81" s="3">
+        <v>16</v>
+      </c>
+      <c r="C81" s="3">
+        <v>13877</v>
+      </c>
+      <c r="D81" s="3"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="3">
+        <v>14425</v>
+      </c>
+      <c r="B82" s="3">
+        <v>18</v>
+      </c>
+      <c r="C82" s="3">
+        <v>0</v>
+      </c>
+      <c r="D82" s="3"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="3">
+        <v>14490</v>
+      </c>
+      <c r="B83" s="3">
+        <v>79</v>
+      </c>
+      <c r="C83" s="3">
+        <v>10423</v>
+      </c>
+      <c r="D83" s="3"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="3">
+        <v>14552</v>
+      </c>
+      <c r="B84" s="3">
+        <v>31</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D84" s="3"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="3">
+        <v>14569</v>
+      </c>
+      <c r="B85" s="3">
+        <v>52</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D85" s="3"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="3">
+        <v>14630</v>
+      </c>
+      <c r="B86" s="3">
+        <v>60</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D86" s="3"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="3">
+        <v>14634</v>
+      </c>
+      <c r="B87" s="3">
+        <v>66</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D87" s="3"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="3">
+        <v>14685</v>
+      </c>
+      <c r="B88" s="3">
+        <v>51</v>
+      </c>
+      <c r="C88" s="3">
+        <v>14552</v>
+      </c>
+      <c r="D88" s="3"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="3">
+        <v>14746</v>
+      </c>
+      <c r="B89" s="3">
+        <v>69</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D89" s="3"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="3">
+        <v>14762</v>
+      </c>
+      <c r="B90" s="3">
+        <v>48</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D90" s="3"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="3">
+        <v>14788</v>
+      </c>
+      <c r="B91" s="3">
+        <v>29</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D91" s="3"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="3">
+        <v>14801</v>
+      </c>
+      <c r="B92" s="3">
+        <v>24</v>
+      </c>
+      <c r="C92" s="3">
+        <v>0</v>
+      </c>
+      <c r="D92" s="3"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="3">
+        <v>14812</v>
+      </c>
+      <c r="B93" s="3">
+        <v>22</v>
+      </c>
+      <c r="C93" s="3">
+        <v>0</v>
+      </c>
+      <c r="D93" s="3"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="3">
+        <v>14833</v>
+      </c>
+      <c r="B94" s="3">
+        <v>80</v>
+      </c>
+      <c r="C94" s="3">
+        <v>13877</v>
+      </c>
+      <c r="D94" s="3"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="3">
+        <v>14867</v>
+      </c>
+      <c r="B95" s="3">
+        <v>69</v>
+      </c>
+      <c r="C95" s="3">
+        <v>0</v>
+      </c>
+      <c r="D95" s="3"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="3">
+        <v>14964</v>
+      </c>
+      <c r="B96" s="3">
+        <v>82</v>
+      </c>
+      <c r="C96" s="3">
+        <v>0</v>
+      </c>
+      <c r="D96" s="3"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="3">
+        <v>15030</v>
+      </c>
+      <c r="B97" s="3">
+        <v>85</v>
+      </c>
+      <c r="C97" s="3">
+        <v>0</v>
+      </c>
+      <c r="D97" s="3"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="3">
+        <v>15058</v>
+      </c>
+      <c r="B98" s="3">
+        <v>27</v>
+      </c>
+      <c r="C98" s="3">
+        <v>0</v>
+      </c>
+      <c r="D98" s="3"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="3">
+        <v>15078</v>
+      </c>
+      <c r="B99" s="3">
+        <v>20</v>
+      </c>
+      <c r="C99" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C77" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" s="3">
-        <v>14115</v>
-      </c>
-      <c r="B78" s="3">
-        <v>25</v>
-      </c>
-      <c r="C78" s="3">
-        <v>11930</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" s="3">
-        <v>14187</v>
-      </c>
-      <c r="B79" s="3">
-        <v>42</v>
-      </c>
-      <c r="C79" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" s="3">
-        <v>14187</v>
-      </c>
-      <c r="B80" s="3">
-        <v>80</v>
-      </c>
-      <c r="C80" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" s="3">
-        <v>14255</v>
-      </c>
-      <c r="B81" s="3">
-        <v>93</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="3">
-        <v>14301</v>
-      </c>
-      <c r="B82" s="3">
-        <v>81</v>
-      </c>
-      <c r="C82" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="3">
-        <v>14336</v>
-      </c>
-      <c r="B83" s="3">
-        <v>16</v>
-      </c>
-      <c r="C83" s="3">
-        <v>13877</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" s="3">
-        <v>14425</v>
-      </c>
-      <c r="B84" s="3">
-        <v>18</v>
-      </c>
-      <c r="C84" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" s="3">
-        <v>14490</v>
-      </c>
-      <c r="B85" s="3">
-        <v>79</v>
-      </c>
-      <c r="C85" s="3">
-        <v>10423</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" s="3">
-        <v>14552</v>
-      </c>
-      <c r="B86" s="3">
-        <v>31</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="3">
-        <v>14569</v>
-      </c>
-      <c r="B87" s="3">
-        <v>52</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="3">
-        <v>14630</v>
-      </c>
-      <c r="B88" s="3">
-        <v>60</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" s="3">
-        <v>14634</v>
-      </c>
-      <c r="B89" s="3">
-        <v>66</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="3">
-        <v>14685</v>
-      </c>
-      <c r="B90" s="3">
-        <v>51</v>
-      </c>
-      <c r="C90" s="3">
-        <v>14552</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" s="3">
-        <v>14746</v>
-      </c>
-      <c r="B91" s="3">
-        <v>69</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" s="3">
-        <v>14762</v>
-      </c>
-      <c r="B92" s="3">
-        <v>48</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="3">
-        <v>14788</v>
-      </c>
-      <c r="B93" s="3">
-        <v>29</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="3">
-        <v>14801</v>
-      </c>
-      <c r="B94" s="3">
-        <v>24</v>
-      </c>
-      <c r="C94" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="3">
-        <v>14812</v>
-      </c>
-      <c r="B95" s="3">
-        <v>22</v>
-      </c>
-      <c r="C95" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="3">
-        <v>14833</v>
-      </c>
-      <c r="B96" s="3">
-        <v>80</v>
-      </c>
-      <c r="C96" s="3">
-        <v>13877</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" s="3">
-        <v>14867</v>
-      </c>
-      <c r="B97" s="3">
-        <v>69</v>
-      </c>
-      <c r="C97" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" s="3">
-        <v>14964</v>
-      </c>
-      <c r="B98" s="3">
-        <v>82</v>
-      </c>
-      <c r="C98" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" s="3">
-        <v>15030</v>
-      </c>
-      <c r="B99" s="3">
-        <v>85</v>
-      </c>
-      <c r="C99" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A100" s="3">
-        <v>15058</v>
-      </c>
-      <c r="B100" s="3">
-        <v>27</v>
-      </c>
-      <c r="C100" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A101" s="3">
-        <v>15078</v>
-      </c>
-      <c r="B101" s="3">
-        <v>20</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="D99" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>